<commit_message>
employee_view methode voor tien rijkste, dashboard employee uitgecomment
</commit_message>
<xml_diff>
--- a/Requirements en User Stories/stappen_door_klikken.xlsx
+++ b/Requirements en User Stories/stappen_door_klikken.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Make IT work\team-2\Requirements en User Stories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eendkonijn/Google Drive/A Make René Work/Project Sofa/Requirements en User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90D3E52C-4C93-4996-95F2-8101E3FA4682}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="18000" windowHeight="9360" xr2:uid="{CB67E798-AB35-4678-BF69-5D391E3D2F79}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,51 +135,51 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -192,70 +194,70 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Goed" xfId="1" builtinId="26"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -290,7 +292,7 @@
         <xdr:cNvPr id="2" name="Connector: Elbow 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0732FEB2-E8ED-41A4-B234-EC948D0A4CD3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0732FEB2-E8ED-41A4-B234-EC948D0A4CD3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -345,7 +347,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A2C5417-BE25-4C8D-940A-4641FF00CCAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1A2C5417-BE25-4C8D-940A-4641FF00CCAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -395,7 +397,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FDB9C8A-FFF2-4A65-8C34-887750F2D505}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8FDB9C8A-FFF2-4A65-8C34-887750F2D505}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -448,7 +450,7 @@
         <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD903F6E-498A-4995-B7B0-D3DA3CE31FA4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD903F6E-498A-4995-B7B0-D3DA3CE31FA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -501,7 +503,7 @@
         <xdr:cNvPr id="6" name="Connector: Elbow 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27862EF9-5515-48C1-B679-1D7BE8CAE5B4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{27862EF9-5515-48C1-B679-1D7BE8CAE5B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -556,7 +558,7 @@
         <xdr:cNvPr id="7" name="Connector: Elbow 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89F7FFE6-87B5-4B60-A575-D9246D58CC3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89F7FFE6-87B5-4B60-A575-D9246D58CC3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -611,7 +613,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6AAF3C1-2BD4-401F-AFC3-C05FE4C8E52E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C6AAF3C1-2BD4-401F-AFC3-C05FE4C8E52E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -664,7 +666,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A15E97B-E007-4598-B379-07CADFDA7A33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A15E97B-E007-4598-B379-07CADFDA7A33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -717,7 +719,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A57DC59A-B4EC-4A79-A7BA-3E609364CFA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A57DC59A-B4EC-4A79-A7BA-3E609364CFA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -767,7 +769,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6CC244D-D70C-47BB-AFFD-DF29B9D49AA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6CC244D-D70C-47BB-AFFD-DF29B9D49AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -820,7 +822,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84564A25-3FD2-4356-A5F0-D1111FF42E99}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84564A25-3FD2-4356-A5F0-D1111FF42E99}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -873,7 +875,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CEAA9B4-11F0-496B-A7DC-E3BA27F63EE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4CEAA9B4-11F0-496B-A7DC-E3BA27F63EE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -926,7 +928,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6782E60-0673-4B75-B2C2-15EE9F3754FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D6782E60-0673-4B75-B2C2-15EE9F3754FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -979,7 +981,7 @@
         <xdr:cNvPr id="15" name="Connector: Elbow 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25FD2A23-849A-4FCB-8359-DC80AB530CFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{25FD2A23-849A-4FCB-8359-DC80AB530CFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1034,7 +1036,7 @@
         <xdr:cNvPr id="16" name="Connector: Elbow 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1211117D-AC21-4752-AA7F-93AF1F614B63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1211117D-AC21-4752-AA7F-93AF1F614B63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1089,7 +1091,7 @@
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{136A7D55-BFE9-40B2-9F1B-ED3FC4D8020C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{136A7D55-BFE9-40B2-9F1B-ED3FC4D8020C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1142,7 +1144,7 @@
         <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F336842-7740-4A9D-A053-880B96C49EFC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F336842-7740-4A9D-A053-880B96C49EFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1195,7 +1197,7 @@
         <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76585166-96D2-40F0-9857-F43584DC7502}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{76585166-96D2-40F0-9857-F43584DC7502}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1529,166 +1531,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98B47E1-3FE8-4123-963E-2319B7930674}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G5" s="22" t="s">
+    <row r="5" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="G5" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E7" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G9" s="20" t="s">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="G9" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G10" s="19"/>
-    </row>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="5:12" x14ac:dyDescent="0.2">
       <c r="L11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E13" s="18" t="s">
+    <row r="13" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E13" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="8"/>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E16" s="8"/>
-      <c r="G16" s="12" t="s">
+    <row r="14" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E15" s="14"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E16" s="14"/>
+      <c r="G16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E17" s="8"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E19" s="8"/>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E17" s="14"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E19" s="14"/>
       <c r="I19" s="16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E20" s="8"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="8"/>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E23" s="8"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E20" s="14"/>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E21" s="14"/>
+      <c r="I21" s="18"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E23" s="14"/>
       <c r="K23" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="13"/>
-      <c r="E24" s="8"/>
-      <c r="G24" s="12" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C24" s="4"/>
+      <c r="E24" s="14"/>
+      <c r="G24" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="11"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E25" s="8"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="8"/>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E25" s="14"/>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E26" s="14"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E28" s="14"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E32" s="4" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E32" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="3" t="s">
+    <row r="37" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G37" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="2"/>
-    </row>
-    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G38" s="7"/>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G40" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G9:G10"/>
     <mergeCell ref="G37:G38"/>
     <mergeCell ref="G24:G26"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="E13:E29"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G9:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
client_view_employee werkt nog beter
</commit_message>
<xml_diff>
--- a/Requirements en User Stories/stappen_door_klikken.xlsx
+++ b/Requirements en User Stories/stappen_door_klikken.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Uitlog</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>/index</t>
-  </si>
-  <si>
-    <t>/employee_view Overzicht Employee</t>
   </si>
   <si>
     <t xml:space="preserve">/dashboard Overzicht gekozen rekening </t>
@@ -78,6 +75,19 @@
   </si>
   <si>
     <t>/new_account          Klant worden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/dashboard Ov gekozen rekening </t>
+  </si>
+  <si>
+    <t>/employee_view_mkb
+Overzicht voor hoofd MKB</t>
+  </si>
+  <si>
+    <t>/employee_view_particulieren Overzicht voor hoofd Employee</t>
+  </si>
+  <si>
+    <t>/client_view_employee</t>
   </si>
 </sst>
 </file>
@@ -191,7 +201,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -203,6 +213,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -231,27 +271,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -292,7 +311,7 @@
         <xdr:cNvPr id="2" name="Connector: Elbow 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0732FEB2-E8ED-41A4-B234-EC948D0A4CD3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0732FEB2-E8ED-41A4-B234-EC948D0A4CD3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -347,7 +366,7 @@
         <xdr:cNvPr id="3" name="Straight Connector 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1A2C5417-BE25-4C8D-940A-4641FF00CCAC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A2C5417-BE25-4C8D-940A-4641FF00CCAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -397,7 +416,7 @@
         <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8FDB9C8A-FFF2-4A65-8C34-887750F2D505}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FDB9C8A-FFF2-4A65-8C34-887750F2D505}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -450,7 +469,7 @@
         <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD903F6E-498A-4995-B7B0-D3DA3CE31FA4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD903F6E-498A-4995-B7B0-D3DA3CE31FA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -503,7 +522,7 @@
         <xdr:cNvPr id="6" name="Connector: Elbow 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{27862EF9-5515-48C1-B679-1D7BE8CAE5B4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27862EF9-5515-48C1-B679-1D7BE8CAE5B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -558,7 +577,7 @@
         <xdr:cNvPr id="7" name="Connector: Elbow 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89F7FFE6-87B5-4B60-A575-D9246D58CC3B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89F7FFE6-87B5-4B60-A575-D9246D58CC3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -613,7 +632,7 @@
         <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C6AAF3C1-2BD4-401F-AFC3-C05FE4C8E52E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6AAF3C1-2BD4-401F-AFC3-C05FE4C8E52E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -666,7 +685,7 @@
         <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A15E97B-E007-4598-B379-07CADFDA7A33}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A15E97B-E007-4598-B379-07CADFDA7A33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -719,7 +738,7 @@
         <xdr:cNvPr id="10" name="Straight Connector 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A57DC59A-B4EC-4A79-A7BA-3E609364CFA6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A57DC59A-B4EC-4A79-A7BA-3E609364CFA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -769,7 +788,7 @@
         <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6CC244D-D70C-47BB-AFFD-DF29B9D49AA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6CC244D-D70C-47BB-AFFD-DF29B9D49AA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -822,7 +841,7 @@
         <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84564A25-3FD2-4356-A5F0-D1111FF42E99}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84564A25-3FD2-4356-A5F0-D1111FF42E99}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -875,7 +894,7 @@
         <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4CEAA9B4-11F0-496B-A7DC-E3BA27F63EE3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CEAA9B4-11F0-496B-A7DC-E3BA27F63EE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -928,7 +947,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D6782E60-0673-4B75-B2C2-15EE9F3754FF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6782E60-0673-4B75-B2C2-15EE9F3754FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -981,7 +1000,7 @@
         <xdr:cNvPr id="15" name="Connector: Elbow 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{25FD2A23-849A-4FCB-8359-DC80AB530CFB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25FD2A23-849A-4FCB-8359-DC80AB530CFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1036,7 +1055,7 @@
         <xdr:cNvPr id="16" name="Connector: Elbow 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1211117D-AC21-4752-AA7F-93AF1F614B63}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1211117D-AC21-4752-AA7F-93AF1F614B63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1076,22 +1095,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
+      <xdr:colOff>660400</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>85727</xdr:rowOff>
+      <xdr:rowOff>187328</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{136A7D55-BFE9-40B2-9F1B-ED3FC4D8020C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{136A7D55-BFE9-40B2-9F1B-ED3FC4D8020C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1099,8 +1118,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5753100" y="3838575"/>
-          <a:ext cx="809625" cy="828677"/>
+          <a:off x="6604000" y="4635500"/>
+          <a:ext cx="647700" cy="123828"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1144,7 +1163,7 @@
         <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F336842-7740-4A9D-A053-880B96C49EFC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F336842-7740-4A9D-A053-880B96C49EFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1197,7 +1216,7 @@
         <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{76585166-96D2-40F0-9857-F43584DC7502}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76585166-96D2-40F0-9857-F43584DC7502}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1207,6 +1226,271 @@
         <a:xfrm>
           <a:off x="661987" y="5641183"/>
           <a:ext cx="435769" cy="47623"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>631825</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84564A25-3FD2-4356-A5F0-D1111FF42E99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3733800" y="3835400"/>
+          <a:ext cx="619125" cy="1565275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>69851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>669925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{136A7D55-BFE9-40B2-9F1B-ED3FC4D8020C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6604000" y="4832351"/>
+          <a:ext cx="657225" cy="603249"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2184400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{136A7D55-BFE9-40B2-9F1B-ED3FC4D8020C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6578600" y="5461000"/>
+          <a:ext cx="635000" cy="203200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{136A7D55-BFE9-40B2-9F1B-ED3FC4D8020C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7886700" y="4965700"/>
+          <a:ext cx="0" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{136A7D55-BFE9-40B2-9F1B-ED3FC4D8020C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7886700" y="4914900"/>
+          <a:ext cx="12700" cy="495300"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1535,145 +1819,160 @@
   <dimension ref="A5:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19:I21"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.83203125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="12" max="12" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E7" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="G6" s="20"/>
-    </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E7" s="16" t="s">
+    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="G9" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E13" s="23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E14" s="24"/>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E15" s="24"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E16" s="24"/>
+      <c r="G16" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E17" s="24"/>
+      <c r="G17" s="20"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E18" s="24"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E20" s="24"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E23" s="24"/>
+      <c r="K23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="4"/>
+      <c r="E24" s="24"/>
+      <c r="G24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E8" s="18"/>
-    </row>
-    <row r="9" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="G9" s="21" t="s">
-        <v>12</v>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E25" s="24"/>
+      <c r="G25" s="19"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E26" s="24"/>
+      <c r="G26" s="20"/>
+      <c r="I26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E27" s="24"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E28" s="24"/>
+      <c r="G28" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="10" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="L11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E13" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E14" s="14"/>
-    </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E15" s="14"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E16" s="14"/>
-      <c r="G16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E17" s="14"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E19" s="14"/>
-      <c r="I19" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E20" s="14"/>
-      <c r="I20" s="17"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E21" s="14"/>
-      <c r="I21" s="18"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E23" s="14"/>
-      <c r="K23" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C24" s="4"/>
-      <c r="E24" s="14"/>
-      <c r="G24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E25" s="14"/>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E26" s="14"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E28" s="14"/>
-    </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E29" s="15"/>
+      <c r="E29" s="25"/>
+      <c r="G29" s="19"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="21" t="s">
         <v>3</v>
       </c>
+      <c r="G30" s="20"/>
+      <c r="I30" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C31" s="12"/>
+      <c r="C31" s="22"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E32" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="I32" s="8"/>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G37" s="6" t="s">
+      <c r="G37" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G38" s="7"/>
+      <c r="G38" s="17"/>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G40" s="1" t="s">
@@ -1681,16 +1980,17 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="I19:I21"/>
+  <mergeCells count="10">
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E13:E29"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="I16:I18"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="G37:G38"/>
     <mergeCell ref="G24:G26"/>
     <mergeCell ref="G16:G17"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E13:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
stappen_door_klikken bijgewerkt met nieuwe paginaflow
</commit_message>
<xml_diff>
--- a/Requirements en User Stories/stappen_door_klikken.xlsx
+++ b/Requirements en User Stories/stappen_door_klikken.xlsx
@@ -50,9 +50,6 @@
     <t>/index</t>
   </si>
   <si>
-    <t xml:space="preserve">/dashboard Overzicht gekozen rekening </t>
-  </si>
-  <si>
     <t>/pay</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>/new_account          Klant worden</t>
   </si>
   <si>
-    <t xml:space="preserve">/dashboard Ov gekozen rekening </t>
-  </si>
-  <si>
     <t>/employee_view_mkb
 Overzicht voor hoofd MKB</t>
   </si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>/client_view_employee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/dashboard_employee gekozen rekening </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/dashboard_client Overzicht gekozen rekening </t>
   </si>
 </sst>
 </file>
@@ -1154,9 +1154,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1171,8 +1171,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5753100" y="3019425"/>
-          <a:ext cx="819150" cy="790575"/>
+          <a:off x="6591300" y="3019425"/>
+          <a:ext cx="622300" cy="219075"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1819,7 +1819,7 @@
   <dimension ref="A5:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1832,23 +1832,23 @@
   <sheetData>
     <row r="5" spans="5:12" x14ac:dyDescent="0.2">
       <c r="G5" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E7" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E7" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="8" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E8" s="11"/>
     </row>
     <row r="9" spans="5:12" x14ac:dyDescent="0.2">
       <c r="G9" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="5:12" x14ac:dyDescent="0.2">
@@ -1856,12 +1856,12 @@
     </row>
     <row r="11" spans="5:12" x14ac:dyDescent="0.2">
       <c r="L11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E13" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="5:12" x14ac:dyDescent="0.2">
@@ -1874,13 +1874,13 @@
     <row r="16" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E16" s="24"/>
       <c r="G16" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1907,17 +1907,17 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E23" s="24"/>
       <c r="K23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="4"/>
       <c r="E24" s="24"/>
       <c r="G24" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J24" s="3"/>
     </row>
@@ -1937,7 +1937,7 @@
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="E28" s="24"/>
       <c r="G28" s="18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1953,7 +1953,7 @@
       </c>
       <c r="G30" s="20"/>
       <c r="I30" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>